<commit_message>
DE223800: upload templates missing mandatory asterisk
</commit_message>
<xml_diff>
--- a/database/files/prof/business-upload/corp_adjustments_upload_template.xlsx
+++ b/database/files/prof/business-upload/corp_adjustments_upload_template.xlsx
@@ -42,13 +42,13 @@
     </r>
   </si>
   <si>
-    <t>Country Name</t>
+    <t>*Country Name</t>
   </si>
   <si>
-    <t>Sales Territory Code</t>
+    <t>*Sales Territory Code</t>
   </si>
   <si>
-    <t>SCMS Value</t>
+    <t>*SCMS Value</t>
   </si>
 </sst>
 </file>

</xml_diff>